<commit_message>
Improved letter and circle experiments (v3), and some other prototypes.
</commit_message>
<xml_diff>
--- a/v3/conditions_v3.xlsx
+++ b/v3/conditions_v3.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>condition</t>
   </si>
@@ -29,6 +29,15 @@
     <t>group</t>
   </si>
   <si>
+    <t>color_1</t>
+  </si>
+  <si>
+    <t>color_2</t>
+  </si>
+  <si>
+    <t>agency_level</t>
+  </si>
+  <si>
     <t>A</t>
   </si>
   <si>
@@ -38,18 +47,42 @@
     <t>explicit</t>
   </si>
   <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
     <t>C</t>
   </si>
   <si>
     <t>implicit</t>
   </si>
   <si>
+    <t>green</t>
+  </si>
+  <si>
     <t>D</t>
   </si>
   <si>
     <t>free</t>
   </si>
   <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>grey</t>
+  </si>
+  <si>
+    <t>purple</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
     <t>F</t>
   </si>
   <si>
@@ -57,6 +90,9 @@
   </si>
   <si>
     <t>invalid</t>
+  </si>
+  <si>
+    <t>white</t>
   </si>
   <si>
     <t>W</t>
@@ -180,7 +216,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -188,9 +224,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1320,7 +1353,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1333,7 +1366,8 @@
     <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.3516" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.3516" style="1" customWidth="1"/>
+    <col min="9" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.55" customHeight="1">
@@ -1352,312 +1386,431 @@
       <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="F1" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="5">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s" s="5">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s" s="5">
-        <v>7</v>
-      </c>
-      <c r="E2" s="4">
+      <c r="B2" t="s" s="4">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s" s="4">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s" s="4">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3">
         <v>1</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="F2" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s" s="4">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" ht="20.35" customHeight="1">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s" s="7">
+      <c r="B3" t="s" s="6">
         <v>8</v>
       </c>
-      <c r="D3" t="s" s="7">
-        <v>9</v>
-      </c>
-      <c r="E3" s="6">
+      <c r="C3" t="s" s="6">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E3" s="5">
         <v>2</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="F3" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s" s="6">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s" s="7">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s" s="7">
-        <v>11</v>
-      </c>
-      <c r="E4" s="6">
+      <c r="B4" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="E4" s="5">
         <v>3</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+      <c r="F4" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s" s="6">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s" s="7">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s" s="7">
-        <v>11</v>
-      </c>
-      <c r="E5" s="6">
+      <c r="B5" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="E5" s="5">
         <v>3</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="F5" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="H5" t="s" s="6">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s" s="7">
+      <c r="B6" t="s" s="6">
         <v>8</v>
       </c>
-      <c r="D6" t="s" s="7">
-        <v>9</v>
-      </c>
-      <c r="E6" s="6">
+      <c r="C6" t="s" s="6">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E6" s="5">
         <v>2</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="F6" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s" s="6">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="E7" s="6">
+      <c r="B7" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s" s="6">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="E7" s="5">
         <v>1</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="F7" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s" s="6">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" t="s" s="7">
+      <c r="B8" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s" s="6">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s" s="6">
+        <v>25</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s" s="6">
         <v>12</v>
       </c>
-      <c r="C8" t="s" s="7">
+      <c r="G8" t="s" s="6">
+        <v>26</v>
+      </c>
+      <c r="H8" t="s" s="6">
         <v>13</v>
       </c>
-      <c r="D8" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
     </row>
     <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" t="s" s="7">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s" s="7">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="E9" s="6">
+      <c r="B9" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s" s="6">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5">
         <v>0</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="F9" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="G9" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s" s="6">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="E10" s="6">
+      <c r="B10" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s" s="6">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="E10" s="5">
         <v>1</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="F10" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s" s="6">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="C11" t="s" s="7">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="E11" s="6">
+      <c r="B11" t="s" s="6">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s" s="6">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s" s="6">
+        <v>25</v>
+      </c>
+      <c r="E11" s="5">
         <v>0</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="F11" t="s" s="6">
+        <v>26</v>
+      </c>
+      <c r="G11" t="s" s="6">
+        <v>26</v>
+      </c>
+      <c r="H11" t="s" s="6">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" ht="20.35" customHeight="1">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" t="s" s="7">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s" s="7">
-        <v>18</v>
-      </c>
-      <c r="D12" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="E12" s="6">
+      <c r="B12" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s" s="6">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s" s="6">
+        <v>25</v>
+      </c>
+      <c r="E12" s="5">
         <v>0</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="F12" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s" s="6">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s" s="7">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s" s="7">
-        <v>11</v>
-      </c>
-      <c r="E13" s="6">
+      <c r="B13" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="E13" s="5">
         <v>3</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="F13" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s" s="6">
+        <v>26</v>
+      </c>
+      <c r="H13" t="s" s="6">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s" s="7">
+      <c r="B14" t="s" s="6">
         <v>8</v>
       </c>
-      <c r="D14" t="s" s="7">
-        <v>9</v>
-      </c>
-      <c r="E14" s="6">
+      <c r="C14" t="s" s="6">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E14" s="5">
         <v>2</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="F14" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="H14" t="s" s="6">
+        <v>22</v>
+      </c>
     </row>
     <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s" s="7">
+      <c r="B15" t="s" s="6">
         <v>8</v>
       </c>
-      <c r="D15" t="s" s="7">
-        <v>9</v>
-      </c>
-      <c r="E15" s="6">
+      <c r="C15" t="s" s="6">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E15" s="5">
         <v>2</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="F15" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="H15" t="s" s="6">
+        <v>13</v>
+      </c>
     </row>
     <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" s="6">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s" s="7">
+      <c r="B16" t="s" s="6">
         <v>8</v>
       </c>
-      <c r="D16" t="s" s="7">
-        <v>9</v>
-      </c>
-      <c r="E16" s="6">
-        <v>3</v>
-      </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="C16" t="s" s="6">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="E16" s="5">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="H16" t="s" s="6">
+        <v>22</v>
+      </c>
     </row>
     <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" s="6">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="E17" s="6">
+      <c r="B17" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s" s="6">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="E17" s="5">
         <v>1</v>
       </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+      <c r="F17" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="H17" t="s" s="6">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>

<commit_message>
Improve v3 intro images
</commit_message>
<xml_diff>
--- a/v3/conditions_v3.xlsx
+++ b/v3/conditions_v3.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
     <t>condition</t>
   </si>
@@ -29,6 +29,12 @@
     <t>group</t>
   </si>
   <si>
+    <t>char_color_1</t>
+  </si>
+  <si>
+    <t>char_color_2</t>
+  </si>
+  <si>
     <t>color_1</t>
   </si>
   <si>
@@ -47,55 +53,55 @@
     <t>explicit</t>
   </si>
   <si>
+    <t>yellow</t>
+  </si>
+  <si>
     <t>red</t>
   </si>
   <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>implicit</t>
+  </si>
+  <si>
     <t>blue</t>
   </si>
   <si>
-    <t>high</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>implicit</t>
+    <t>D</t>
+  </si>
+  <si>
+    <t>free</t>
+  </si>
+  <si>
+    <t>white</t>
   </si>
   <si>
     <t>green</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>free</t>
-  </si>
-  <si>
-    <t>yellow</t>
+    <t>low</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>purple</t>
   </si>
   <si>
     <t>grey</t>
-  </si>
-  <si>
-    <t>purple</t>
-  </si>
-  <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>invalid</t>
-  </si>
-  <si>
-    <t>white</t>
-  </si>
-  <si>
-    <t>W</t>
   </si>
   <si>
     <t>E</t>
@@ -1353,7 +1359,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1367,7 +1373,9 @@
     <col min="6" max="6" width="16.3516" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.3516" style="1" customWidth="1"/>
     <col min="8" max="8" width="16.3516" style="1" customWidth="1"/>
-    <col min="9" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.3516" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.3516" style="1" customWidth="1"/>
+    <col min="11" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.55" customHeight="1">
@@ -1395,31 +1403,43 @@
       <c r="H1" t="s" s="2">
         <v>7</v>
       </c>
+      <c r="I1" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s" s="2">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" ht="20.55" customHeight="1">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s" s="4">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s" s="4">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
       </c>
       <c r="F2" t="s" s="4">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s" s="4">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="I2" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s" s="4">
+        <v>15</v>
       </c>
     </row>
     <row r="3" ht="20.35" customHeight="1">
@@ -1427,25 +1447,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="s" s="6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s" s="6">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s" s="6">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" s="5">
         <v>2</v>
       </c>
       <c r="F3" t="s" s="6">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s" s="6">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s" s="6">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="I3" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s" s="6">
+        <v>15</v>
       </c>
     </row>
     <row r="4" ht="20.35" customHeight="1">
@@ -1453,25 +1479,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="s" s="6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s" s="6">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s" s="6">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E4" s="5">
         <v>3</v>
       </c>
       <c r="F4" t="s" s="6">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s" s="6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s" s="6">
         <v>13</v>
+      </c>
+      <c r="I4" t="s" s="6">
+        <v>13</v>
+      </c>
+      <c r="J4" t="s" s="6">
+        <v>15</v>
       </c>
     </row>
     <row r="5" ht="20.35" customHeight="1">
@@ -1479,25 +1511,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s" s="6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s" s="6">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s" s="6">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E5" s="5">
         <v>3</v>
       </c>
       <c r="F5" t="s" s="6">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s" s="6">
         <v>21</v>
       </c>
-      <c r="H5" t="s" s="6">
-        <v>22</v>
+      <c r="I5" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="J5" t="s" s="6">
+        <v>23</v>
       </c>
     </row>
     <row r="6" ht="20.35" customHeight="1">
@@ -1505,25 +1543,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="s" s="6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s" s="6">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s" s="6">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E6" s="5">
         <v>2</v>
       </c>
       <c r="F6" t="s" s="6">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s" s="6">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H6" t="s" s="6">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="I6" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s" s="6">
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="20.35" customHeight="1">
@@ -1531,25 +1575,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s" s="6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s" s="6">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s" s="6">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E7" s="5">
         <v>1</v>
       </c>
       <c r="F7" t="s" s="6">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G7" t="s" s="6">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H7" t="s" s="6">
-        <v>22</v>
+        <v>14</v>
+      </c>
+      <c r="I7" t="s" s="6">
+        <v>14</v>
+      </c>
+      <c r="J7" t="s" s="6">
+        <v>23</v>
       </c>
     </row>
     <row r="8" ht="20.35" customHeight="1">
@@ -1557,25 +1607,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="s" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s" s="6">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s" s="6">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" s="5">
         <v>0</v>
       </c>
       <c r="F8" t="s" s="6">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="G8" t="s" s="6">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H8" t="s" s="6">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="I8" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="J8" t="s" s="6">
+        <v>15</v>
       </c>
     </row>
     <row r="9" ht="20.35" customHeight="1">
@@ -1583,25 +1639,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="s" s="6">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s" s="6">
         <v>27</v>
       </c>
       <c r="D9" t="s" s="6">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
       </c>
       <c r="F9" t="s" s="6">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="G9" t="s" s="6">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="H9" t="s" s="6">
         <v>22</v>
+      </c>
+      <c r="I9" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="J9" t="s" s="6">
+        <v>23</v>
       </c>
     </row>
     <row r="10" ht="20.35" customHeight="1">
@@ -1609,25 +1671,31 @@
         <v>9</v>
       </c>
       <c r="B10" t="s" s="6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s" s="6">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s" s="6">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E10" s="5">
         <v>1</v>
       </c>
       <c r="F10" t="s" s="6">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G10" t="s" s="6">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="H10" t="s" s="6">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="I10" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="J10" t="s" s="6">
+        <v>15</v>
       </c>
     </row>
     <row r="11" ht="20.35" customHeight="1">
@@ -1635,25 +1703,31 @@
         <v>10</v>
       </c>
       <c r="B11" t="s" s="6">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s" s="6">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s" s="6">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E11" s="5">
         <v>0</v>
       </c>
       <c r="F11" t="s" s="6">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G11" t="s" s="6">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H11" t="s" s="6">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="I11" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="J11" t="s" s="6">
+        <v>15</v>
       </c>
     </row>
     <row r="12" ht="20.35" customHeight="1">
@@ -1661,25 +1735,31 @@
         <v>11</v>
       </c>
       <c r="B12" t="s" s="6">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s" s="6">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s" s="6">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E12" s="5">
         <v>0</v>
       </c>
       <c r="F12" t="s" s="6">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="G12" t="s" s="6">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="H12" t="s" s="6">
         <v>22</v>
+      </c>
+      <c r="I12" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="J12" t="s" s="6">
+        <v>23</v>
       </c>
     </row>
     <row r="13" ht="20.35" customHeight="1">
@@ -1687,25 +1767,31 @@
         <v>12</v>
       </c>
       <c r="B13" t="s" s="6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s" s="6">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s" s="6">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E13" s="5">
         <v>3</v>
       </c>
       <c r="F13" t="s" s="6">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G13" t="s" s="6">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H13" t="s" s="6">
         <v>13</v>
+      </c>
+      <c r="I13" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="J13" t="s" s="6">
+        <v>15</v>
       </c>
     </row>
     <row r="14" ht="20.35" customHeight="1">
@@ -1713,25 +1799,31 @@
         <v>13</v>
       </c>
       <c r="B14" t="s" s="6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s" s="6">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s" s="6">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E14" s="5">
         <v>2</v>
       </c>
       <c r="F14" t="s" s="6">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G14" t="s" s="6">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H14" t="s" s="6">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="I14" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="J14" t="s" s="6">
+        <v>23</v>
       </c>
     </row>
     <row r="15" ht="20.35" customHeight="1">
@@ -1739,25 +1831,31 @@
         <v>14</v>
       </c>
       <c r="B15" t="s" s="6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s" s="6">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s" s="6">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E15" s="5">
         <v>2</v>
       </c>
       <c r="F15" t="s" s="6">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G15" t="s" s="6">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H15" t="s" s="6">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="I15" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="J15" t="s" s="6">
+        <v>15</v>
       </c>
     </row>
     <row r="16" ht="20.35" customHeight="1">
@@ -1765,25 +1863,31 @@
         <v>15</v>
       </c>
       <c r="B16" t="s" s="6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s" s="6">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s" s="6">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E16" s="5">
         <v>2</v>
       </c>
       <c r="F16" t="s" s="6">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G16" t="s" s="6">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H16" t="s" s="6">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="I16" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="J16" t="s" s="6">
+        <v>23</v>
       </c>
     </row>
     <row r="17" ht="20.35" customHeight="1">
@@ -1791,25 +1895,31 @@
         <v>16</v>
       </c>
       <c r="B17" t="s" s="6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s" s="6">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D17" t="s" s="6">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E17" s="5">
         <v>1</v>
       </c>
       <c r="F17" t="s" s="6">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G17" t="s" s="6">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H17" t="s" s="6">
-        <v>22</v>
+        <v>14</v>
+      </c>
+      <c r="I17" t="s" s="6">
+        <v>14</v>
+      </c>
+      <c r="J17" t="s" s="6">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>